<commit_message>
New and improved report
</commit_message>
<xml_diff>
--- a/bin/Debug/ZSOX report template.xlsx
+++ b/bin/Debug/ZSOX report template.xlsx
@@ -306,7 +306,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <protection hidden="1"/>
@@ -326,16 +326,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -357,6 +347,21 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -375,15 +380,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -700,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,19 +720,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="21" t="s">
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="22"/>
-      <c r="O1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="24"/>
     </row>
     <row r="2" spans="1:17" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -746,13 +747,13 @@
       <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="9" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="6" t="s">
@@ -767,91 +768,173 @@
       <c r="K2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="O10" s="2"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Added tab & file totals to report
</commit_message>
<xml_diff>
--- a/bin/Debug/ZSOX report template.xlsx
+++ b/bin/Debug/ZSOX report template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Missing lines of information</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -159,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -226,19 +229,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -291,6 +281,58 @@
     <border>
       <left/>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -306,7 +348,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <protection hidden="1"/>
@@ -338,7 +380,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -347,10 +389,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -362,29 +404,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -693,7 +738,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -701,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,27 +759,28 @@
     <col min="3" max="3" width="14.5703125" style="4" customWidth="1"/>
     <col min="4" max="4" width="11.140625" style="4"/>
     <col min="5" max="5" width="32.5703125" style="4" customWidth="1"/>
-    <col min="6" max="14" width="11.140625" style="4"/>
-    <col min="15" max="15" width="34.5703125" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="11.140625" style="4"/>
+    <col min="6" max="15" width="11.140625" style="4"/>
+    <col min="16" max="16" width="34.5703125" style="4" customWidth="1"/>
+    <col min="17" max="16384" width="11.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G1" s="19" t="s">
+    <row r="1" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="22" t="s">
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="23"/>
-      <c r="O1" s="24"/>
-    </row>
-    <row r="2" spans="1:17" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="22"/>
+      <c r="P1" s="23"/>
+    </row>
+    <row r="2" spans="1:18" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -771,19 +817,22 @@
       <c r="L2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="P2" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
-      <c r="B3" s="25"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -797,10 +846,11 @@
       <c r="M3" s="15"/>
       <c r="N3" s="15"/>
       <c r="O3" s="15"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P3" s="15"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
-      <c r="B4" s="26"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -814,10 +864,11 @@
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P4" s="17"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
-      <c r="B5" s="26"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -831,10 +882,11 @@
       <c r="M5" s="17"/>
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P5" s="17"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
-      <c r="B6" s="26"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -848,8 +900,9 @@
       <c r="M6" s="17"/>
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
@@ -865,8 +918,9 @@
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
       <c r="O7" s="18"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P7" s="18"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
@@ -882,8 +936,9 @@
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
       <c r="O8" s="18"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P8" s="18"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -899,8 +954,9 @@
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
       <c r="O9" s="18"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P9" s="18"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
@@ -916,10 +972,11 @@
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
       <c r="O10" s="18"/>
-      <c r="P10" s="2"/>
+      <c r="P10" s="18"/>
       <c r="Q10" s="2"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -935,11 +992,12 @@
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
       <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="G1:L1"/>
-    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="G1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>